<commit_message>
Modified fetch_compartments_to_variablesTF.py and changed Networking to Network
</commit_message>
<xml_diff>
--- a/oci_tools/automation_toolkit/example/CD3-ManagementServices-template.xlsx
+++ b/oci_tools/automation_toolkit/example/CD3-ManagementServices-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\oci_develop_new\oci_tenancy\SetUpOCI_Via_TF\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\oci_develop_new\oci_tools\automation_toolkit\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -43848,8 +43848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC129"/>
   <sheetViews>
-    <sheetView topLeftCell="K13" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Pushed for Modules - alarms, events, notifications
</commit_message>
<xml_diff>
--- a/oci_tools/automation_toolkit/example/CD3-ManagementServices-template.xlsx
+++ b/oci_tools/automation_toolkit/example/CD3-ManagementServices-template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22990" windowHeight="8280" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22990" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -3986,12 +3986,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -5924,7 +5924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -5949,7 +5949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -5966,15 +5966,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="89.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
@@ -6405,7 +6405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="I72" sqref="I72"/>
     </sheetView>
   </sheetViews>
@@ -6429,20 +6429,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="85.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="24"/>
     </row>
     <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
@@ -9133,7 +9133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
@@ -9210,10 +9210,10 @@
       <c r="L2" s="7" t="s">
         <v>655</v>
       </c>
-      <c r="M2" s="24" t="s">
+      <c r="M2" s="21" t="s">
         <v>656</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="21" t="s">
         <v>7</v>
       </c>
       <c r="O2" s="12"/>

</xml_diff>